<commit_message>
rill-analysis: Apply luopan project
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/test-luopan.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/test-luopan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -228,6 +228,14 @@
   </si>
   <si>
     <t>dummy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>example/type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -235,7 +243,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +293,23 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -477,7 +502,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -547,7 +572,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -809,11 +840,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62081664"/>
-        <c:axId val="71229824"/>
+        <c:axId val="77898880"/>
+        <c:axId val="77900416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62081664"/>
+        <c:axId val="77898880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,14 +853,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71229824"/>
+        <c:crossAx val="77900416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71229824"/>
+        <c:axId val="77900416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,7 +869,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62081664"/>
+        <c:crossAx val="77898880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -856,7 +887,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000555" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000555" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -898,8 +929,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G13" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A8:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G14" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A8:G14"/>
   <tableColumns count="7">
     <tableColumn id="1" name="参数" dataDxfId="6"/>
     <tableColumn id="2" name="名称" dataDxfId="5"/>
@@ -1202,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1227,24 +1258,24 @@
     <col min="20" max="20" width="5.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" ht="3.75" customHeight="1">
       <c r="O1" s="5"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="B2" s="23" t="str">
+      <c r="B2" s="25" t="str">
         <f>_input!$B2&amp;_input!$B3&amp;"趋势图"</f>
         <v>搜索+推广点击消费趋势图</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="2:15">
       <c r="O3" s="5"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="2" t="str">
+      <c r="B4" s="23" t="str">
         <f>_input!$B3</f>
         <v>点击消费</v>
       </c>
@@ -1326,9 +1357,9 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1489,6 +1520,24 @@
         <v>42</v>
       </c>
       <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="18" t="str">
+        <f>$B10</f>
+        <v>dateType</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
rill-analysis: Refactor parameter component construct logic and remove onChange Listener, and add support iframe embedded.
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/test-luopan.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/test-luopan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -244,6 +244,10 @@
   </si>
   <si>
     <t>{0}{1}{2}报表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calendar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -520,71 +524,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -848,11 +852,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="69356160"/>
-        <c:axId val="79483264"/>
+        <c:axId val="79831040"/>
+        <c:axId val="79832576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69356160"/>
+        <c:axId val="79831040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,14 +865,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79483264"/>
+        <c:crossAx val="79832576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79483264"/>
+        <c:axId val="79832576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -877,7 +881,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69356160"/>
+        <c:crossAx val="79831040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -895,7 +899,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000006" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000006" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000666" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000666" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1241,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1267,7 +1271,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="3.75" customHeight="1">
-      <c r="O1" s="5"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="2:15">
       <c r="B2" s="25" t="str">
@@ -1277,78 +1281,78 @@
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
-      <c r="O2" s="5"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="O3" s="5"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="23" t="str">
+      <c r="B4" s="22" t="str">
         <f>_input!$B3</f>
         <v>点击消费</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="O4" s="5"/>
+      <c r="O4" s="4"/>
     </row>
     <row r="5" spans="2:15" ht="3" customHeight="1">
-      <c r="O5" s="5"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="2:15">
-      <c r="O6" s="5"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" spans="2:15">
-      <c r="O7" s="5"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="O8" s="5"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="2:15">
-      <c r="O9" s="5"/>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="2:15">
-      <c r="O10" s="5"/>
+      <c r="O10" s="4"/>
     </row>
     <row r="11" spans="2:15">
-      <c r="O11" s="5"/>
+      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="2:15">
-      <c r="O12" s="5"/>
+      <c r="O12" s="4"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="O13" s="5"/>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="O14" s="5"/>
+      <c r="O14" s="4"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="O15" s="5"/>
+      <c r="O15" s="4"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="O16" s="5"/>
+      <c r="O16" s="4"/>
     </row>
     <row r="17" spans="15:15">
-      <c r="O17" s="5"/>
+      <c r="O17" s="4"/>
     </row>
     <row r="18" spans="15:15">
-      <c r="O18" s="5"/>
+      <c r="O18" s="4"/>
     </row>
     <row r="19" spans="15:15">
-      <c r="O19" s="5"/>
+      <c r="O19" s="4"/>
     </row>
     <row r="20" spans="15:15">
-      <c r="O20" s="5"/>
+      <c r="O20" s="4"/>
     </row>
     <row r="21" spans="15:15">
-      <c r="O21" s="5"/>
+      <c r="O21" s="4"/>
     </row>
     <row r="22" spans="15:15">
-      <c r="O22" s="5"/>
+      <c r="O22" s="4"/>
     </row>
     <row r="23" spans="15:15">
-      <c r="O23" s="5"/>
+      <c r="O23" s="4"/>
     </row>
     <row r="24" spans="15:15">
-      <c r="O24" s="5"/>
+      <c r="O24" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1367,7 +1371,7 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1384,67 +1388,67 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="19" t="b">
+      <c r="B4" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1452,48 +1456,48 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16" t="s">
+      <c r="E11" s="16"/>
+      <c r="F11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1503,14 +1507,14 @@
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16" t="s">
+      <c r="E12" s="16"/>
+      <c r="F12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1520,46 +1524,46 @@
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="17" t="str">
+      <c r="E13" s="16" t="str">
         <f t="shared" ref="E13" si="0">$B12</f>
         <v>lineId</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="18" t="str">
+      <c r="E14" s="17" t="str">
         <f>$B10</f>
         <v>dateType</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="18" t="str">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="17" t="str">
         <f>$B12&amp;" "&amp;$B13&amp;" "&amp;$B14</f>
         <v>lineId indId showType</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="15" t="s">
+      <c r="F15" s="23"/>
+      <c r="G15" s="14" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1589,7 +1593,7 @@
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1">
@@ -1622,50 +1626,50 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="24">
         <v>3344110</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="24">
         <v>3544111</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="24">
         <v>3444111</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="24">
         <v>3344111</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="24">
         <v>3744111</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.25" thickBot="1">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="24">
         <v>4444111</v>
       </c>
     </row>

</xml_diff>